<commit_message>
100 runs and batch size tests done
</commit_message>
<xml_diff>
--- a/error/new/signals_layer_impact/signals.xlsx
+++ b/error/new/signals_layer_impact/signals.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
@@ -164,26 +164,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -202,8 +182,1519 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="9"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1layer_training</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$B$3:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.650000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>98.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>99.82</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>99.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99.78</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>99.68</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99.98</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>99.92</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99.99</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99.86</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99.99</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1layer_validation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$C$3:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.150000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79.95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>81.69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82.84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>84.16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>84.65</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.44</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.07</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>86.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>86.89</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>86.84</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>86.28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>86.05</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>88.06</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>87.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2layers_training</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$E$3:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99.71</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99.97</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>99.96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>99.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99.98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>99.93</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99.92</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>99.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99.95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99.93</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99.99</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000014-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>2layers_validation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$F$3:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92.83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91.33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93.27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>93.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>93.85</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93.45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94.87</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>93.57</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>93.73</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>92.78</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>94.34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>94.29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95.05</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>95.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000015-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>3layers_training</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$K$3:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99.87</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99.77</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>99.91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>99.96</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>99.82</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99.93</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>99.96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99.84</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99.84</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99.99</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>3layers_validation</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$L$3:$L$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>89.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91.18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>92.71</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91.18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>92.37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92.14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92.96</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>92.22</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>93.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>94.31</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>93.55</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>92.07</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>94.16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>94.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>4layers_training</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$N$3:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99.98</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99.37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>99.93</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>99.98</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99.86</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>99.99</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99.87</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>99.87</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99.96</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99.92</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000018-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>4layers_validation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$O$3:$O$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94.72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95.23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96.12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94.11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96.48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93.78</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97.02</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>96.68</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96.99</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>96.94</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>96.79</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>96.76</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>95.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000019-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>stop_citeria</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$Q$3:$Q$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>97.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001A-324D-4F6D-AEDF-060127A43006}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="9"/>
           <c:tx>
             <c:v>1layer_training</c:v>
           </c:tx>
@@ -369,13 +1860,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8FC8-471A-9A12-00903AC5CB98}"/>
+              <c16:uniqueId val="{00000001-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="10"/>
           <c:tx>
             <c:v>1layer_validation</c:v>
           </c:tx>
@@ -538,13 +2029,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8FC8-471A-9A12-00903AC5CB98}"/>
+              <c16:uniqueId val="{00000003-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="11"/>
           <c:tx>
             <c:v>2layers_training</c:v>
           </c:tx>
@@ -710,13 +2201,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8FC8-471A-9A12-00903AC5CB98}"/>
+              <c16:uniqueId val="{00000005-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="12"/>
           <c:tx>
             <c:v>2layers_validation</c:v>
           </c:tx>
@@ -879,13 +2370,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8FC8-471A-9A12-00903AC5CB98}"/>
+              <c16:uniqueId val="{00000007-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="13"/>
           <c:tx>
             <c:v>3layers_training</c:v>
           </c:tx>
@@ -1051,13 +2542,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-8FC8-471A-9A12-00903AC5CB98}"/>
+              <c16:uniqueId val="{00000009-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="14"/>
           <c:tx>
             <c:v>3layers_validation</c:v>
           </c:tx>
@@ -1220,13 +2711,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-8FC8-471A-9A12-00903AC5CB98}"/>
+              <c16:uniqueId val="{0000000B-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:order val="15"/>
           <c:tx>
             <c:v>4layers_training</c:v>
           </c:tx>
@@ -1392,13 +2883,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-8FC8-471A-9A12-00903AC5CB98}"/>
+              <c16:uniqueId val="{0000000D-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:order val="16"/>
           <c:tx>
             <c:v>4layers_validation</c:v>
           </c:tx>
@@ -1561,13 +3052,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-8FC8-471A-9A12-00903AC5CB98}"/>
+              <c16:uniqueId val="{0000000F-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
-          <c:order val="8"/>
+          <c:order val="17"/>
           <c:tx>
             <c:v>stop_citeria</c:v>
           </c:tx>
@@ -1733,7 +3224,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2A4F-4839-949A-9BD05D3DA6CD}"/>
+              <c16:uniqueId val="{00000011-324D-4F6D-AEDF-060127A43006}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1819,26 +3310,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1954,26 +3425,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2010,13 +3461,6 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -2083,560 +3527,1209 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="1"/>
+              <a:t>Impact</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="1" baseline="0"/>
+              <a:t> of using many convolutional layers in a high-level feature dataset</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8208315131109287E-2"/>
+          <c:y val="7.4293339347466542E-2"/>
+          <c:w val="0.80170337300530259"/>
+          <c:h val="0.83307347068761195"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1layer_training</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$B$3:$B$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$B$3,Folha1!$B$7,Folha1!$B$11,Folha1!$B$15,Folha1!$B$19,Folha1!$B$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1layer_validation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$C$3:$C$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$C$3,Folha1!$C$7,Folha1!$C$11,Folha1!$C$15,Folha1!$C$19,Folha1!$C$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2layers_training</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$E$3:$E$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$E$3,Folha1!$E$7,Folha1!$E$11,Folha1!$E$15,Folha1!$E$19,Folha1!$E$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>2layers_validation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$F$3:$F$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$F$3,Folha1!$F$7,Folha1!$F$11,Folha1!$F$15,Folha1!$F$19,Folha1!$F$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>3layers_training</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$K$3:$K$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$K$3,Folha1!$K$7,Folha1!$K$11,Folha1!$K$15,Folha1!$K$19,Folha1!$K$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>3layers_validation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$L$3:$L$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$L$3,Folha1!$L$7,Folha1!$L$11,Folha1!$L$15,Folha1!$L$19,Folha1!$L$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>4layers_training</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$N$3:$N$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$N$3,Folha1!$N$7,Folha1!$N$11,Folha1!$N$15,Folha1!$N$19,Folha1!$N$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>4layers_validation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$O$3:$O$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$O$3,Folha1!$O$7,Folha1!$O$11,Folha1!$O$15,Folha1!$O$19,Folha1!$O$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="399"/>
+        <c:axId val="396743360"/>
+        <c:axId val="396744672"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>stop_citeria</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="3175" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3,Folha1!$A$7,Folha1!$A$11,Folha1!$A$15,Folha1!$A$19,Folha1!$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$Q$3:$Q$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$Q$3,Folha1!$Q$7,Folha1!$Q$11,Folha1!$Q$15,Folha1!$Q$19,Folha1!$Q$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-5C1F-4C81-9AC8-B5B155D7BD2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="396743360"/>
+        <c:axId val="396744672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="396743360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" b="1"/>
+                  <a:t>Epochs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="396744672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="396744672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" b="1"/>
+                  <a:t>Accuracy (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="396743360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2644,15 +4737,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:colOff>106680</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>181792</xdr:rowOff>
+      <xdr:rowOff>67492</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
+      <xdr:colOff>396240</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>172648</xdr:rowOff>
+      <xdr:rowOff>58348</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2672,6 +4765,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>150876</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02C7BFD0-F290-42D1-B4E3-0A8B0A7BF2C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2945,8 +5076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V52" sqref="V52"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>